<commit_message>
Add Vuelta 2023, bar_plot and final confusion matrix
</commit_message>
<xml_diff>
--- a/Data/Data_2023.xlsx
+++ b/Data/Data_2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Violeau Pierre\Data_Science\Breakaway_win\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685759C9-C5CE-4928-B031-F4A25A82892C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AB59DE-B42E-4EE1-AA10-AAE6D8FE928B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -390,8 +390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="107" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="107" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L59" sqref="L59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1889,13 +1889,13 @@
         <v>2</v>
       </c>
       <c r="D40">
-        <v>181.3</v>
+        <v>182</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G40">
         <v>1</v>
@@ -1904,13 +1904,16 @@
         <v>0</v>
       </c>
       <c r="I40">
-        <v>113</v>
+        <v>2</v>
       </c>
       <c r="J40">
         <v>1</v>
       </c>
       <c r="K40">
-        <v>2619</v>
+        <v>2754</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -1947,6 +1950,9 @@
       <c r="K41">
         <v>3486</v>
       </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -1982,6 +1988,9 @@
       <c r="K42">
         <v>1798</v>
       </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -2017,6 +2026,9 @@
       <c r="K43">
         <v>2384</v>
       </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -2052,6 +2064,9 @@
       <c r="K44">
         <v>3976</v>
       </c>
+      <c r="L44">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -2087,6 +2102,9 @@
       <c r="K45">
         <v>987</v>
       </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -2122,6 +2140,9 @@
       <c r="K46">
         <v>3611</v>
       </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -2157,6 +2178,9 @@
       <c r="K47">
         <v>2972</v>
       </c>
+      <c r="L47">
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -2192,8 +2216,11 @@
       <c r="K48">
         <v>2215</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -2227,8 +2254,11 @@
       <c r="K49">
         <v>888</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -2262,8 +2292,11 @@
       <c r="K50">
         <v>4282</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>14</v>
       </c>
@@ -2297,8 +2330,11 @@
       <c r="K51">
         <v>4655</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>14</v>
       </c>
@@ -2315,10 +2351,10 @@
         <v>0</v>
       </c>
       <c r="F52">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -2330,10 +2366,13 @@
         <v>1</v>
       </c>
       <c r="K52">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2494</v>
+      </c>
+      <c r="L52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>14</v>
       </c>
@@ -2367,8 +2406,11 @@
       <c r="K53">
         <v>2089</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -2402,8 +2444,11 @@
       <c r="K54">
         <v>3303</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>14</v>
       </c>
@@ -2437,8 +2482,11 @@
       <c r="K55">
         <v>4624</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>14</v>
       </c>
@@ -2472,8 +2520,11 @@
       <c r="K56">
         <v>935</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>14</v>
       </c>
@@ -2507,8 +2558,11 @@
       <c r="K57">
         <v>4330</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -2541,6 +2595,9 @@
       </c>
       <c r="K58">
         <v>854</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>